<commit_message>
Improve student import functionality by adding a download link for import template and clear instructions, addressing previous import failures due to missing fields.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 9f6f5aa9-e739-4b3f-b6c7-8a0a1554b32f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/5dbbb00f-656a-4fa7-b435-2e7b2a79b6d7/3fd73927-296d-4dd6-8007-5f9d6ed41580.jpg
</commit_message>
<xml_diff>
--- a/client/public/student_import_template.xlsx
+++ b/client/public/student_import_template.xlsx
@@ -3,8 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Instructions" sheetId="1" r:id="rId1"/>
-    <sheet name="Template" sheetId="2" r:id="rId2"/>
+    <sheet name="Students" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -398,119 +397,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Student Import Template</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Instructions:</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>1. Fill in the required fields: firstName, lastName, username, email, and password</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>2. Optional fields: gradeLevel, section, and houseId</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>3. Do not modify the column headers in the template sheet</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>4. Save this file as .xlsx or .csv before uploading</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>5. For houseId, use the numeric ID of the house (visible in the Houses management page)</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>Notes:</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>- Usernames must be unique</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>- Emails must be valid format and unique</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>- Passwords should be at least 8 characters</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>Sample Houses:</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>1 - Phoenix</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>2 - Dragon</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>3 - Griffin</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>4 - Sphinx</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A19"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -552,10 +452,10 @@
         <v>john.smith@school.edu</v>
       </c>
       <c r="E2" t="str">
-        <v>password123</v>
+        <v>Password123</v>
       </c>
       <c r="F2" t="str">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G2" t="str">
         <v>A</v>
@@ -578,47 +478,21 @@
         <v>jane.doe@school.edu</v>
       </c>
       <c r="E3" t="str">
-        <v>password123</v>
+        <v>Password123</v>
       </c>
       <c r="F3" t="str">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G3" t="str">
         <v>B</v>
       </c>
       <c r="H3" t="str">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Michael</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Johnson</v>
-      </c>
-      <c r="C4" t="str">
-        <v>michael.j</v>
-      </c>
-      <c r="D4" t="str">
-        <v>michael.j@school.edu</v>
-      </c>
-      <c r="E4" t="str">
-        <v>password123</v>
-      </c>
-      <c r="F4" t="str">
-        <v>8</v>
-      </c>
-      <c r="G4" t="str">
-        <v>C</v>
-      </c>
-      <c r="H4" t="str">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>